<commit_message>
8 october updated the importData documentation
</commit_message>
<xml_diff>
--- a/Protein name and abbreviations.xlsx
+++ b/Protein name and abbreviations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/dorsa_sohaei_mail_utoronto_ca/Documents/Documents/UofT/MSc/Experiments/Freedman/Autoantibody Preliminary/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityhealthnetwork-my.sharepoint.com/personal/lisa_avery_uhnresearch_ca/Documents/PDscreen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E74A1066-6712-4375-A305-EF2CFB2BBF0A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{E74A1066-6712-4375-A305-EF2CFB2BBF0A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C856D14B-4C6A-40AF-9E84-590BB71E5297}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{10C84448-0180-4E9A-9532-C1EA3132B4CB}"/>
+    <workbookView xWindow="6420" yWindow="360" windowWidth="14630" windowHeight="10200" xr2:uid="{10C84448-0180-4E9A-9532-C1EA3132B4CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2526" uniqueCount="2521">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2528" uniqueCount="2523">
   <si>
     <t>Mucin-16 OS=Homo sapiens OX=9606 GN=MUC16 PE=1 SV=3 - [MUC16_HUMAN]</t>
   </si>
@@ -7597,6 +7597,12 @@
   </si>
   <si>
     <t>IGLC3</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Description</t>
   </si>
 </sst>
 </file>
@@ -7978,14 +7984,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F77F776F-286F-4CE8-820E-1C44CE84E225}">
-  <dimension ref="B3:C1265"/>
+  <dimension ref="B2:C1265"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>2521</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2522</v>
+      </c>
+    </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>2520</v>

</xml_diff>